<commit_message>
add test to cbcdairyil
</commit_message>
<xml_diff>
--- a/Projects/CBCDAIRYIL/Tests/Data/test_case_data.xlsx
+++ b/Projects/CBCDAIRYIL/Tests/Data/test_case_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">matches!$A$1:$J$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
@@ -45,6 +45,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$B$1:$P$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$B$1:$P$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$B$1:$P$2</definedName>
@@ -67,6 +69,8 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$B$1:$P$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$B$1:$P$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$B$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$B$1:$P$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$B$1:$P$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -78,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
   <si>
     <t xml:space="preserve">probe_match_fk</t>
   </si>
@@ -255,6 +259,9 @@
   </si>
   <si>
     <t xml:space="preserve">test case 2 – bath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test case 3 – min 2 facing</t>
   </si>
   <si>
     <t xml:space="preserve">probe_group_id</t>
@@ -359,7 +366,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,6 +380,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,29 +488,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,7 +1144,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>8</v>
@@ -1142,22 +1153,22 @@
         <v>1</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17" s="1" t="n">
         <v>1</v>
@@ -1168,15 +1179,15 @@
       </c>
       <c r="L17" s="0" t="n">
         <f aca="false">H17</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
@@ -1194,21 +1205,181 @@
         <v>1</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="0" t="n">
         <f aca="false">B18</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L18" s="0" t="n">
         <f aca="false">H18</f>
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">B19</f>
+        <v>9</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">H19</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">B20</f>
+        <v>10</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <f aca="false">H20</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">B21</f>
+        <v>10</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <f aca="false">H21</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">B22</f>
+        <v>10</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <f aca="false">H22</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1232,68 +1403,68 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1334,7 +1505,7 @@
       <c r="L2" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="M2" s="5" t="n">
+      <c r="M2" s="6" t="n">
         <v>7290102394845</v>
       </c>
       <c r="N2" s="0" t="s">
@@ -1378,7 +1549,7 @@
       <c r="L3" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="6" t="n">
         <v>7290102397730</v>
       </c>
       <c r="N3" s="0" t="s">
@@ -1422,7 +1593,7 @@
       <c r="L4" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="6" t="n">
         <v>7290102396665</v>
       </c>
       <c r="N4" s="0" t="s">
@@ -1466,7 +1637,7 @@
       <c r="L5" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="6" t="n">
         <v>7290102394463</v>
       </c>
       <c r="N5" s="0" t="s">
@@ -1495,7 +1666,7 @@
       <c r="G6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="5"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1534,7 +1705,7 @@
       <c r="L7" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="M7" s="5" t="n">
+      <c r="M7" s="6" t="n">
         <v>7290102395224</v>
       </c>
       <c r="N7" s="0" t="s">
@@ -1578,7 +1749,7 @@
       <c r="L8" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="M8" s="5" t="n">
+      <c r="M8" s="6" t="n">
         <v>7290102395231</v>
       </c>
       <c r="N8" s="0" t="s">
@@ -1622,14 +1793,14 @@
       <c r="L9" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="M9" s="5" t="n">
+      <c r="M9" s="6" t="n">
         <v>7290102396399</v>
       </c>
       <c r="N9" s="0" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1646,34 +1817,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.6224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="49.4081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,1450 +1896,1535 @@
       <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>22</v>
       </c>
       <c r="V1" s="0" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B2,matches!$H$2:$H$200,$C2)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B2,matches!$H$2:$H$200,$C2, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B2,matches!$H$2:$H$200,$C2)</f>
-        <v>3</v>
-      </c>
-      <c r="H2" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B2,matches!$H$2:$H$200,$C2, matches!$F$2:$F$200, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="I2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7" t="s">
+    <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B2,matches!$H$2:$H$199,$C2)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B2,matches!$H$2:$H$199,$C2, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B2,matches!$H$2:$H$199,$C2)</f>
+        <v>3</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B2,matches!$H$2:$H$199,$C2, matches!$F$2:$F$199, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="I2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="7" t="str">
+      <c r="L2" s="8" t="str">
         <f aca="false">VLOOKUP(C2,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 1</v>
       </c>
-      <c r="M2" s="7" t="str">
+      <c r="M2" s="8" t="str">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N2" s="7" t="n">
+      <c r="N2" s="8" t="n">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O2" s="7" t="n">
+      <c r="O2" s="8" t="n">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P2" s="7" t="str">
+      <c r="P2" s="8" t="str">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q2" s="7" t="str">
+      <c r="Q2" s="8" t="str">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yellow cheeses lite shelf</v>
       </c>
-      <c r="R2" s="7" t="n">
+      <c r="R2" s="8" t="n">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$L$40, 9, 0)</f>
         <v>169</v>
       </c>
-      <c r="S2" s="7" t="str">
+      <c r="S2" s="8" t="str">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T2" s="7" t="str">
+      <c r="T2" s="8" t="str">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U2" s="7" t="n">
+      <c r="U2" s="8" t="n">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V2" s="7" t="n">
+      <c r="V2" s="8" t="n">
         <f aca="false">VLOOKUP($C2, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102394845</v>
       </c>
     </row>
-    <row r="3" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B3,matches!$H$2:$H$200,$C3)</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B3,matches!$H$2:$H$200,$C3, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B3,matches!$H$2:$H$200,$C3)</f>
+    <row r="3" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B3,matches!$H$2:$H$199,$C3)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B3,matches!$H$2:$H$199,$C3, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B3,matches!$H$2:$H$199,$C3)</f>
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B3,matches!$H$2:$H$200,$C3, matches!$F$2:$F$200, 1)</f>
+      <c r="H3" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B3,matches!$H$2:$H$199,$C3, matches!$F$2:$F$199, 1)</f>
         <v>4</v>
       </c>
-      <c r="I3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="7" t="s">
+      <c r="I3" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="7" t="str">
+      <c r="L3" s="8" t="str">
         <f aca="false">VLOOKUP(C3,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 2</v>
       </c>
-      <c r="M3" s="7" t="str">
+      <c r="M3" s="8" t="str">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N3" s="7" t="n">
+      <c r="N3" s="8" t="n">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O3" s="7" t="n">
+      <c r="O3" s="8" t="n">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P3" s="7" t="str">
+      <c r="P3" s="8" t="str">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q3" s="7" t="str">
+      <c r="Q3" s="8" t="str">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Standard yellow cheeses and shelf</v>
       </c>
-      <c r="R3" s="7" t="n">
+      <c r="R3" s="8" t="n">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$L$40, 9, 0)</f>
         <v>144</v>
       </c>
-      <c r="S3" s="7" t="str">
+      <c r="S3" s="8" t="str">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T3" s="7" t="str">
+      <c r="T3" s="8" t="str">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U3" s="7" t="n">
+      <c r="U3" s="8" t="n">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V3" s="7" t="n">
+      <c r="V3" s="8" t="n">
         <f aca="false">VLOOKUP($C3, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102397730</v>
       </c>
     </row>
-    <row r="4" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B4,matches!$H$2:$H$200,$C4)</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B4,matches!$H$2:$H$200,$C4, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B4,matches!$H$2:$H$200,$C4)</f>
+    <row r="4" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B4,matches!$H$2:$H$199,$C4)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B4,matches!$H$2:$H$199,$C4, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B4,matches!$H$2:$H$199,$C4)</f>
         <v>5</v>
       </c>
-      <c r="H4" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B4,matches!$H$2:$H$200,$C4, matches!$F$2:$F$200, 1)</f>
+      <c r="H4" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B4,matches!$H$2:$H$199,$C4, matches!$F$2:$F$199, 1)</f>
         <v>5</v>
       </c>
-      <c r="I4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="7" t="s">
+      <c r="I4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="7" t="str">
+      <c r="L4" s="8" t="str">
         <f aca="false">VLOOKUP(C4,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 3</v>
       </c>
-      <c r="M4" s="7" t="str">
+      <c r="M4" s="8" t="str">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N4" s="7" t="n">
+      <c r="N4" s="8" t="n">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O4" s="7" t="n">
+      <c r="O4" s="8" t="n">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P4" s="7" t="str">
+      <c r="P4" s="8" t="str">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q4" s="7" t="str">
+      <c r="Q4" s="8" t="str">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yellow cheeses lite shelf</v>
       </c>
-      <c r="R4" s="7" t="n">
+      <c r="R4" s="8" t="n">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$L$40, 9, 0)</f>
         <v>169</v>
       </c>
-      <c r="S4" s="7" t="str">
+      <c r="S4" s="8" t="str">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T4" s="7" t="str">
+      <c r="T4" s="8" t="str">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U4" s="7" t="n">
+      <c r="U4" s="8" t="n">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V4" s="7" t="n">
+      <c r="V4" s="8" t="n">
         <f aca="false">VLOOKUP($C4, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102396665</v>
       </c>
     </row>
-    <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="n">
+    <row r="5" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B5,matches!$H$2:$H$200,$C5)</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B5,matches!$H$2:$H$200,$C5, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B5,matches!$H$2:$H$200,$C5)</f>
+      <c r="E5" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B5,matches!$H$2:$H$199,$C5)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B5,matches!$H$2:$H$199,$C5, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B5,matches!$H$2:$H$199,$C5)</f>
         <v>6</v>
       </c>
-      <c r="H5" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B5,matches!$H$2:$H$200,$C5, matches!$F$2:$F$200, 1)</f>
+      <c r="H5" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B5,matches!$H$2:$H$199,$C5, matches!$F$2:$F$199, 1)</f>
         <v>6</v>
       </c>
-      <c r="I5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="7" t="s">
+      <c r="I5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L5" s="7" t="str">
+      <c r="L5" s="8" t="str">
         <f aca="false">VLOOKUP(C5,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 4</v>
       </c>
-      <c r="M5" s="7" t="str">
+      <c r="M5" s="8" t="str">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N5" s="7" t="n">
+      <c r="N5" s="8" t="n">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O5" s="7" t="n">
+      <c r="O5" s="8" t="n">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P5" s="7" t="str">
+      <c r="P5" s="8" t="str">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q5" s="7" t="str">
+      <c r="Q5" s="8" t="str">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Standard yellow cheeses and shelf</v>
       </c>
-      <c r="R5" s="7" t="n">
+      <c r="R5" s="8" t="n">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$L$40, 9, 0)</f>
         <v>144</v>
       </c>
-      <c r="S5" s="7" t="str">
+      <c r="S5" s="8" t="str">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T5" s="7" t="str">
+      <c r="T5" s="8" t="str">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="U5" s="8" t="n">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V5" s="7" t="n">
+      <c r="V5" s="8" t="n">
         <f aca="false">VLOOKUP($C5, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102394463</v>
       </c>
     </row>
-    <row r="6" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B6,matches!$H$2:$H$200,$C6)</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B6,matches!$H$2:$H$200,$C6, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B6,matches!$H$2:$H$200,$C6)</f>
-        <v>3</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B6,matches!$H$2:$H$200,$C6, matches!$F$2:$F$200, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="I6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7" t="s">
+    <row r="6" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B6,matches!$H$2:$H$199,$C6)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B6,matches!$H$2:$H$199,$C6, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B6,matches!$H$2:$H$199,$C6)</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B6,matches!$H$2:$H$199,$C6, matches!$F$2:$F$199, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="I6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="7" t="str">
+      <c r="L6" s="8" t="str">
         <f aca="false">VLOOKUP(C6,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 1</v>
       </c>
-      <c r="M6" s="7" t="str">
+      <c r="M6" s="8" t="str">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N6" s="7" t="n">
+      <c r="N6" s="8" t="n">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O6" s="7" t="n">
+      <c r="O6" s="8" t="n">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P6" s="7" t="str">
+      <c r="P6" s="8" t="str">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q6" s="7" t="str">
+      <c r="Q6" s="8" t="str">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yellow cheeses lite shelf</v>
       </c>
-      <c r="R6" s="7" t="n">
+      <c r="R6" s="8" t="n">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$L$40, 9, 0)</f>
         <v>169</v>
       </c>
-      <c r="S6" s="7" t="str">
+      <c r="S6" s="8" t="str">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T6" s="7" t="str">
+      <c r="T6" s="8" t="str">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U6" s="7" t="n">
+      <c r="U6" s="8" t="n">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V6" s="7" t="n">
+      <c r="V6" s="8" t="n">
         <f aca="false">VLOOKUP($C6, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102394845</v>
       </c>
     </row>
-    <row r="7" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B7,matches!$H$2:$H$200,$C7)</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B7,matches!$H$2:$H$200,$C7, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B7,matches!$H$2:$H$200,$C7)</f>
+    <row r="7" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B7,matches!$H$2:$H$199,$C7)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B7,matches!$H$2:$H$199,$C7, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B7,matches!$H$2:$H$199,$C7)</f>
         <v>4</v>
       </c>
-      <c r="H7" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B7,matches!$H$2:$H$200,$C7, matches!$F$2:$F$200, 1)</f>
+      <c r="H7" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B7,matches!$H$2:$H$199,$C7, matches!$F$2:$F$199, 1)</f>
         <v>4</v>
       </c>
-      <c r="I7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L7" s="7" t="str">
+      <c r="L7" s="8" t="str">
         <f aca="false">VLOOKUP(C7,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 2</v>
       </c>
-      <c r="M7" s="7" t="str">
+      <c r="M7" s="8" t="str">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N7" s="7" t="n">
+      <c r="N7" s="8" t="n">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O7" s="7" t="n">
+      <c r="O7" s="8" t="n">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P7" s="7" t="str">
+      <c r="P7" s="8" t="str">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q7" s="7" t="str">
+      <c r="Q7" s="8" t="str">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Standard yellow cheeses and shelf</v>
       </c>
-      <c r="R7" s="7" t="n">
+      <c r="R7" s="8" t="n">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$L$40, 9, 0)</f>
         <v>144</v>
       </c>
-      <c r="S7" s="7" t="str">
+      <c r="S7" s="8" t="str">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T7" s="7" t="str">
+      <c r="T7" s="8" t="str">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U7" s="7" t="n">
+      <c r="U7" s="8" t="n">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V7" s="7" t="n">
+      <c r="V7" s="8" t="n">
         <f aca="false">VLOOKUP($C7, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102397730</v>
       </c>
     </row>
-    <row r="8" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B8,matches!$H$2:$H$200,$C8)</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B8,matches!$H$2:$H$200,$C8, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B8,matches!$H$2:$H$200,$C8)</f>
+    <row r="8" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B8,matches!$H$2:$H$199,$C8)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B8,matches!$H$2:$H$199,$C8, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B8,matches!$H$2:$H$199,$C8)</f>
         <v>5</v>
       </c>
-      <c r="H8" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B8,matches!$H$2:$H$200,$C8, matches!$F$2:$F$200, 1)</f>
+      <c r="H8" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B8,matches!$H$2:$H$199,$C8, matches!$F$2:$F$199, 1)</f>
         <v>5</v>
       </c>
-      <c r="I8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="I8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="7" t="str">
+      <c r="L8" s="8" t="str">
         <f aca="false">VLOOKUP(C8,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 3</v>
       </c>
-      <c r="M8" s="7" t="str">
+      <c r="M8" s="8" t="str">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N8" s="7" t="n">
+      <c r="N8" s="8" t="n">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O8" s="7" t="n">
+      <c r="O8" s="8" t="n">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P8" s="7" t="str">
+      <c r="P8" s="8" t="str">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q8" s="7" t="str">
+      <c r="Q8" s="8" t="str">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yellow cheeses lite shelf</v>
       </c>
-      <c r="R8" s="7" t="n">
+      <c r="R8" s="8" t="n">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$L$40, 9, 0)</f>
         <v>169</v>
       </c>
-      <c r="S8" s="7" t="str">
+      <c r="S8" s="8" t="str">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T8" s="7" t="str">
+      <c r="T8" s="8" t="str">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U8" s="7" t="n">
+      <c r="U8" s="8" t="n">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V8" s="7" t="n">
+      <c r="V8" s="8" t="n">
         <f aca="false">VLOOKUP($C8, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102396665</v>
       </c>
     </row>
-    <row r="9" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B9,matches!$H$2:$H$200,$C9)</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B9,matches!$H$2:$H$200,$C9, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B9,matches!$H$2:$H$200,$C9)</f>
-        <v>3</v>
-      </c>
-      <c r="H9" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B9,matches!$H$2:$H$200,$C9, matches!$F$2:$F$200, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7" t="s">
+    <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B9,matches!$H$2:$H$199,$C9)</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B9,matches!$H$2:$H$199,$C9, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B9,matches!$H$2:$H$199,$C9)</f>
+        <v>3</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B9,matches!$H$2:$H$199,$C9, matches!$F$2:$F$199, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L9" s="7" t="str">
+      <c r="L9" s="8" t="str">
         <f aca="false">VLOOKUP(C9,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Product 1</v>
       </c>
-      <c r="M9" s="7" t="str">
+      <c r="M9" s="8" t="str">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yellow Cheese Shelf</v>
       </c>
-      <c r="N9" s="7" t="n">
+      <c r="N9" s="8" t="n">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$G$14, 5, 0)</f>
         <v>35</v>
       </c>
-      <c r="O9" s="7" t="n">
+      <c r="O9" s="8" t="n">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P9" s="7" t="str">
+      <c r="P9" s="8" t="str">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q9" s="7" t="str">
+      <c r="Q9" s="8" t="str">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yellow cheeses lite shelf</v>
       </c>
-      <c r="R9" s="7" t="n">
+      <c r="R9" s="8" t="n">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$L$40, 9, 0)</f>
         <v>169</v>
       </c>
-      <c r="S9" s="7" t="str">
+      <c r="S9" s="8" t="str">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T9" s="7" t="str">
+      <c r="T9" s="8" t="str">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Terra</v>
       </c>
-      <c r="U9" s="7" t="n">
+      <c r="U9" s="8" t="n">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$L$40, 12, 0)</f>
         <v>99</v>
       </c>
-      <c r="V9" s="7" t="n">
+      <c r="V9" s="8" t="n">
         <f aca="false">VLOOKUP($C9, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102394845</v>
       </c>
     </row>
-    <row r="10" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+    <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="E10" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B10,matches!$H$2:$H$200,$C10)</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B10,matches!$H$2:$H$200,$C10, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B10,matches!$H$2:$H$200,$C10)</f>
+      <c r="E10" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B10,matches!$H$2:$H$199,$C10)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B10,matches!$H$2:$H$199,$C10, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B10,matches!$H$2:$H$199,$C10)</f>
         <v>7</v>
       </c>
-      <c r="H10" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B10,matches!$H$2:$H$200,$C10, matches!$F$2:$F$200, 1)</f>
+      <c r="H10" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B10,matches!$H$2:$H$199,$C10, matches!$F$2:$F$199, 1)</f>
         <v>7</v>
       </c>
-      <c r="I10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="7" t="s">
+      <c r="I10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="7" t="str">
+      <c r="L10" s="8" t="str">
         <f aca="false">VLOOKUP(C10,all_products!$A$2:$C$13, 3, 0)</f>
         <v>General Empty</v>
       </c>
-      <c r="M10" s="7" t="str">
+      <c r="M10" s="8" t="str">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$G$14, 4, 0)</f>
         <v>General</v>
       </c>
-      <c r="N10" s="7" t="n">
+      <c r="N10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$G$14, 5, 0)</f>
         <v>0</v>
       </c>
-      <c r="O10" s="7" t="n">
+      <c r="O10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$G$14, 6, 0)</f>
         <v>1</v>
       </c>
-      <c r="P10" s="7" t="str">
+      <c r="P10" s="8" t="str">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Other</v>
       </c>
-      <c r="Q10" s="7" t="n">
+      <c r="Q10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$L$40, 8, 0)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="7" t="n">
+      <c r="R10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$L$40, 9, 0)</f>
         <v>0</v>
       </c>
-      <c r="S10" s="7" t="n">
+      <c r="S10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$L$40, 10, 0)</f>
         <v>0</v>
       </c>
-      <c r="T10" s="7" t="n">
+      <c r="T10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$L$40, 11, 0)</f>
         <v>0</v>
       </c>
-      <c r="U10" s="7" t="n">
+      <c r="U10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$L$40, 12, 0)</f>
         <v>0</v>
       </c>
-      <c r="V10" s="7" t="n">
+      <c r="V10" s="8" t="n">
         <f aca="false">VLOOKUP($C10, all_products!$A$2:$N$45, 13, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+      <c r="A11" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="8" t="n">
         <f aca="false">A11</f>
         <v>5</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="8" t="n">
         <f aca="false">C11</f>
         <v>6</v>
       </c>
-      <c r="E11" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B11,matches!$H$2:$H$200,$C11)</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B11,matches!$H$2:$H$200,$C11, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G11" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B11,matches!$H$2:$H$200,$C11)</f>
-        <v>2</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B11,matches!$H$2:$H$200,$C11, matches!$F$2:$F$200, 1)</f>
-        <v>2</v>
-      </c>
-      <c r="I11" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="7" t="s">
+      <c r="E11" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B11,matches!$H$2:$H$199,$C11)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B11,matches!$H$2:$H$199,$C11, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B11,matches!$H$2:$H$199,$C11)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B11,matches!$H$2:$H$199,$C11, matches!$F$2:$F$199, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L11" s="7" t="str">
+      <c r="L11" s="8" t="str">
         <f aca="false">VLOOKUP(C11,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Muller Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
       </c>
-      <c r="M11" s="7" t="str">
+      <c r="M11" s="8" t="str">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yogurt And White Cups</v>
       </c>
-      <c r="N11" s="7" t="n">
+      <c r="N11" s="8" t="n">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$G$14, 5, 0)</f>
         <v>19</v>
       </c>
-      <c r="O11" s="7" t="n">
+      <c r="O11" s="8" t="n">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P11" s="7" t="str">
+      <c r="P11" s="8" t="str">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q11" s="7" t="str">
+      <c r="Q11" s="8" t="str">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yogurt and white cups</v>
       </c>
-      <c r="R11" s="7" t="n">
+      <c r="R11" s="8" t="n">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$L$40, 9, 0)</f>
         <v>153</v>
       </c>
-      <c r="S11" s="7" t="str">
+      <c r="S11" s="8" t="str">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T11" s="7" t="str">
+      <c r="T11" s="8" t="str">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Muller Natural</v>
       </c>
-      <c r="U11" s="7" t="n">
+      <c r="U11" s="8" t="n">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$L$40, 12, 0)</f>
         <v>98</v>
       </c>
-      <c r="V11" s="7" t="n">
+      <c r="V11" s="8" t="n">
         <f aca="false">VLOOKUP($C11, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102395224</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+      <c r="A12" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="8" t="n">
         <f aca="false">A12</f>
         <v>5</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="8" t="n">
         <f aca="false">C12</f>
         <v>7</v>
       </c>
-      <c r="E12" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B12,matches!$H$2:$H$200,$C12)</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B12,matches!$H$2:$H$200,$C12, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B12,matches!$H$2:$H$200,$C12)</f>
-        <v>3</v>
-      </c>
-      <c r="H12" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B12,matches!$H$2:$H$200,$C12, matches!$F$2:$F$200, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="J12" s="7" t="s">
+      <c r="E12" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B12,matches!$H$2:$H$199,$C12)</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B12,matches!$H$2:$H$199,$C12, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B12,matches!$H$2:$H$199,$C12)</f>
+        <v>3</v>
+      </c>
+      <c r="H12" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B12,matches!$H$2:$H$199,$C12, matches!$F$2:$F$199, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="I12" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="7" t="str">
+      <c r="L12" s="8" t="str">
         <f aca="false">VLOOKUP(C12,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Muller 2.8% Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
       </c>
-      <c r="M12" s="7" t="str">
+      <c r="M12" s="8" t="str">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yogurt And White Cups</v>
       </c>
-      <c r="N12" s="7" t="n">
+      <c r="N12" s="8" t="n">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$G$14, 5, 0)</f>
         <v>19</v>
       </c>
-      <c r="O12" s="7" t="n">
+      <c r="O12" s="8" t="n">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P12" s="7" t="str">
+      <c r="P12" s="8" t="str">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q12" s="7" t="str">
+      <c r="Q12" s="8" t="str">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yogurt and white cups</v>
       </c>
-      <c r="R12" s="7" t="n">
+      <c r="R12" s="8" t="n">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$L$40, 9, 0)</f>
         <v>153</v>
       </c>
-      <c r="S12" s="7" t="str">
+      <c r="S12" s="8" t="str">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T12" s="7" t="str">
+      <c r="T12" s="8" t="str">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Muller Natural</v>
       </c>
-      <c r="U12" s="7" t="n">
+      <c r="U12" s="8" t="n">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$L$40, 12, 0)</f>
         <v>98</v>
       </c>
-      <c r="V12" s="7" t="n">
+      <c r="V12" s="8" t="n">
         <f aca="false">VLOOKUP($C12, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102395231</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="8" t="n">
         <f aca="false">A13</f>
         <v>6</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="8" t="n">
         <f aca="false">C13</f>
         <v>5</v>
       </c>
-      <c r="E13" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B13,matches!$H$2:$H$200,$C13)</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B13,matches!$H$2:$H$200,$C13, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B13,matches!$H$2:$H$200,$C13)</f>
-        <v>3</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B13,matches!$H$2:$H$200,$C13, matches!$F$2:$F$200, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="I13" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="J13" s="7" t="s">
+      <c r="E13" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B13,matches!$H$2:$H$199,$C13)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B13,matches!$H$2:$H$199,$C13, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B13,matches!$H$2:$H$199,$C13)</f>
+        <v>3</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B13,matches!$H$2:$H$199,$C13, matches!$F$2:$F$199, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="I13" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="7" t="str">
+      <c r="L13" s="8" t="str">
         <f aca="false">VLOOKUP(C13,all_products!$A$2:$C$13, 3, 0)</f>
         <v>General Empty</v>
       </c>
-      <c r="M13" s="7" t="str">
+      <c r="M13" s="8" t="str">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$G$14, 4, 0)</f>
         <v>General</v>
       </c>
-      <c r="N13" s="7" t="n">
+      <c r="N13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$G$14, 5, 0)</f>
         <v>0</v>
       </c>
-      <c r="O13" s="7" t="n">
+      <c r="O13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$G$14, 6, 0)</f>
         <v>1</v>
       </c>
-      <c r="P13" s="7" t="str">
+      <c r="P13" s="8" t="str">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Other</v>
       </c>
-      <c r="Q13" s="7" t="n">
+      <c r="Q13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$L$40, 8, 0)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="7" t="n">
+      <c r="R13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$L$40, 9, 0)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="7" t="n">
+      <c r="S13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$L$40, 10, 0)</f>
         <v>0</v>
       </c>
-      <c r="T13" s="7" t="n">
+      <c r="T13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$L$40, 11, 0)</f>
         <v>0</v>
       </c>
-      <c r="U13" s="7" t="n">
+      <c r="U13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$L$40, 12, 0)</f>
         <v>0</v>
       </c>
-      <c r="V13" s="7" t="n">
+      <c r="V13" s="8" t="n">
         <f aca="false">VLOOKUP($C13, all_products!$A$2:$N$45, 13, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="8" t="n">
         <f aca="false">A14</f>
         <v>6</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="8" t="n">
         <f aca="false">C14</f>
         <v>6</v>
       </c>
-      <c r="E14" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B14,matches!$H$2:$H$200,$C14)</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B14,matches!$H$2:$H$200,$C14, matches!$F$2:$F$200, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B14,matches!$H$2:$H$200,$C14)</f>
-        <v>2</v>
-      </c>
-      <c r="H14" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B14,matches!$H$2:$H$200,$C14, matches!$F$2:$F$200, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="7" t="n">
+      <c r="E14" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B14,matches!$H$2:$H$199,$C14)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B14,matches!$H$2:$H$199,$C14, matches!$F$2:$F$199, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B14,matches!$H$2:$H$199,$C14)</f>
+        <v>2</v>
+      </c>
+      <c r="H14" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B14,matches!$H$2:$H$199,$C14, matches!$F$2:$F$199, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="7" t="str">
+      <c r="L14" s="8" t="str">
         <f aca="false">VLOOKUP(C14,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Muller Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
       </c>
-      <c r="M14" s="7" t="str">
+      <c r="M14" s="8" t="str">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yogurt And White Cups</v>
       </c>
-      <c r="N14" s="7" t="n">
+      <c r="N14" s="8" t="n">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$G$14, 5, 0)</f>
         <v>19</v>
       </c>
-      <c r="O14" s="7" t="n">
+      <c r="O14" s="8" t="n">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P14" s="7" t="str">
+      <c r="P14" s="8" t="str">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q14" s="7" t="str">
+      <c r="Q14" s="8" t="str">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yogurt and white cups</v>
       </c>
-      <c r="R14" s="7" t="n">
+      <c r="R14" s="8" t="n">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$L$40, 9, 0)</f>
         <v>153</v>
       </c>
-      <c r="S14" s="7" t="str">
+      <c r="S14" s="8" t="str">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T14" s="7" t="str">
+      <c r="T14" s="8" t="str">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Muller Natural</v>
       </c>
-      <c r="U14" s="7" t="n">
+      <c r="U14" s="8" t="n">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$L$40, 12, 0)</f>
         <v>98</v>
       </c>
-      <c r="V14" s="7" t="n">
+      <c r="V14" s="8" t="n">
         <f aca="false">VLOOKUP($C14, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102395224</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+      <c r="A15" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="8" t="n">
         <f aca="false">A15</f>
         <v>7</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="8" t="n">
         <f aca="false">C15</f>
         <v>5</v>
       </c>
-      <c r="E15" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B15,matches!$H$2:$H$200,$C15)</f>
-        <v>1</v>
-      </c>
-      <c r="F15" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B15,matches!$H$2:$H$200,$C15, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G15" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B15,matches!$H$2:$H$200,$C15)</f>
-        <v>2</v>
-      </c>
-      <c r="H15" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B15,matches!$H$2:$H$200,$C15, matches!$F$2:$F$200, 1)</f>
-        <v>2</v>
-      </c>
-      <c r="I15" s="7" t="n">
+      <c r="E15" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B15,matches!$H$2:$H$199,$C15)</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B15,matches!$H$2:$H$199,$C15, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B15,matches!$H$2:$H$199,$C15)</f>
+        <v>2</v>
+      </c>
+      <c r="H15" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B15,matches!$H$2:$H$199,$C15, matches!$F$2:$F$199, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="I15" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="7" t="str">
+      <c r="L15" s="8" t="str">
         <f aca="false">VLOOKUP(C15,all_products!$A$2:$C$13, 3, 0)</f>
         <v>General Empty</v>
       </c>
-      <c r="M15" s="7" t="str">
+      <c r="M15" s="8" t="str">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$G$14, 4, 0)</f>
         <v>General</v>
       </c>
-      <c r="N15" s="7" t="n">
+      <c r="N15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$G$14, 5, 0)</f>
         <v>0</v>
       </c>
-      <c r="O15" s="7" t="n">
+      <c r="O15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$G$14, 6, 0)</f>
         <v>1</v>
       </c>
-      <c r="P15" s="7" t="str">
+      <c r="P15" s="8" t="str">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Other</v>
       </c>
-      <c r="Q15" s="7" t="n">
+      <c r="Q15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$L$40, 8, 0)</f>
         <v>0</v>
       </c>
-      <c r="R15" s="7" t="n">
+      <c r="R15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$L$40, 9, 0)</f>
         <v>0</v>
       </c>
-      <c r="S15" s="7" t="n">
+      <c r="S15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$L$40, 10, 0)</f>
         <v>0</v>
       </c>
-      <c r="T15" s="7" t="n">
+      <c r="T15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$L$40, 11, 0)</f>
         <v>0</v>
       </c>
-      <c r="U15" s="7" t="n">
+      <c r="U15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$L$40, 12, 0)</f>
         <v>0</v>
       </c>
-      <c r="V15" s="7" t="n">
+      <c r="V15" s="8" t="n">
         <f aca="false">VLOOKUP($C15, all_products!$A$2:$N$45, 13, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
+      <c r="A16" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="8" t="n">
         <f aca="false">A16</f>
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="8" t="n">
         <f aca="false">C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B16,matches!$H$2:$H$200,$C16)</f>
-        <v>1</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B16,matches!$H$2:$H$200,$C16, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B16,matches!$H$2:$H$200,$C16)</f>
-        <v>2</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B16,matches!$H$2:$H$200,$C16, matches!$F$2:$F$200, 1)</f>
-        <v>2</v>
-      </c>
-      <c r="I16" s="7" t="n">
+      <c r="E16" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B16,matches!$H$2:$H$199,$C16)</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B16,matches!$H$2:$H$199,$C16, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B16,matches!$H$2:$H$199,$C16)</f>
+        <v>2</v>
+      </c>
+      <c r="H16" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B16,matches!$H$2:$H$199,$C16, matches!$F$2:$F$199, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="I16" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L16" s="7" t="str">
+      <c r="L16" s="8" t="str">
         <f aca="false">VLOOKUP(C16,all_products!$A$2:$C$13, 3, 0)</f>
         <v>Muller Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
       </c>
-      <c r="M16" s="7" t="str">
+      <c r="M16" s="8" t="str">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yogurt And White Cups</v>
       </c>
-      <c r="N16" s="7" t="n">
+      <c r="N16" s="8" t="n">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$G$14, 5, 0)</f>
         <v>19</v>
       </c>
-      <c r="O16" s="7" t="n">
+      <c r="O16" s="8" t="n">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P16" s="7" t="str">
+      <c r="P16" s="8" t="str">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q16" s="7" t="str">
+      <c r="Q16" s="8" t="str">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yogurt and white cups</v>
       </c>
-      <c r="R16" s="7" t="n">
+      <c r="R16" s="8" t="n">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$L$40, 9, 0)</f>
         <v>153</v>
       </c>
-      <c r="S16" s="7" t="str">
+      <c r="S16" s="8" t="str">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T16" s="7" t="str">
+      <c r="T16" s="8" t="str">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Muller Natural</v>
       </c>
-      <c r="U16" s="7" t="n">
+      <c r="U16" s="8" t="n">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$L$40, 12, 0)</f>
         <v>98</v>
       </c>
-      <c r="V16" s="7" t="n">
+      <c r="V16" s="8" t="n">
         <f aca="false">VLOOKUP($C16, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102395224</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
+      <c r="A17" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8" t="n">
+        <f aca="false">A17</f>
+        <v>9</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <f aca="false">C17</f>
+        <v>6</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B17,matches!$H$2:$H$199,$C17)</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B17,matches!$H$2:$H$199,$C17, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B17,matches!$H$2:$H$199,$C17)</f>
+        <v>6</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B17,matches!$H$2:$H$199,$C17, matches!$F$2:$F$199, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="I17" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="B17" s="7" t="n">
-        <f aca="false">A17</f>
-        <v>8</v>
-      </c>
-      <c r="C17" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="D17" s="7" t="n">
-        <f aca="false">C17</f>
-        <v>7</v>
-      </c>
-      <c r="E17" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B17,matches!$H$2:$H$200,$C17)</f>
-        <v>1</v>
-      </c>
-      <c r="F17" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B17,matches!$H$2:$H$200,$C17, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G17" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B17,matches!$H$2:$H$200,$C17)</f>
-        <v>3</v>
-      </c>
-      <c r="H17" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B17,matches!$H$2:$H$200,$C17, matches!$F$2:$F$200, 1)</f>
-        <v>3</v>
-      </c>
-      <c r="I17" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="J17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="7" t="str">
+      <c r="L17" s="8" t="str">
         <f aca="false">VLOOKUP(C17,all_products!$A$2:$C$13, 3, 0)</f>
-        <v>Muller 2.8% Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
-      </c>
-      <c r="M17" s="7" t="str">
+        <v>Muller Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
+      </c>
+      <c r="M17" s="8" t="str">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$G$14, 4, 0)</f>
         <v>Yogurt And White Cups</v>
       </c>
-      <c r="N17" s="7" t="n">
+      <c r="N17" s="8" t="n">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$G$14, 5, 0)</f>
         <v>19</v>
       </c>
-      <c r="O17" s="7" t="n">
+      <c r="O17" s="8" t="n">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$G$14, 6, 0)</f>
         <v>45</v>
       </c>
-      <c r="P17" s="7" t="str">
+      <c r="P17" s="8" t="str">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$G$14, 7, 0)</f>
         <v>Central Bottling Company</v>
       </c>
-      <c r="Q17" s="7" t="str">
+      <c r="Q17" s="8" t="str">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$L$40, 8, 0)</f>
         <v>Yogurt and white cups</v>
       </c>
-      <c r="R17" s="7" t="n">
+      <c r="R17" s="8" t="n">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$L$40, 9, 0)</f>
         <v>153</v>
       </c>
-      <c r="S17" s="7" t="str">
+      <c r="S17" s="8" t="str">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$L$40, 10, 0)</f>
         <v>SKU</v>
       </c>
-      <c r="T17" s="7" t="str">
+      <c r="T17" s="8" t="str">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$L$40, 11, 0)</f>
         <v>Muller Natural</v>
       </c>
-      <c r="U17" s="7" t="n">
+      <c r="U17" s="8" t="n">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$L$40, 12, 0)</f>
         <v>98</v>
       </c>
-      <c r="V17" s="7" t="n">
+      <c r="V17" s="8" t="n">
         <f aca="false">VLOOKUP($C17, all_products!$A$2:$N$45, 13, 0)</f>
+        <v>7290102395224</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B18" s="8" t="n">
+        <f aca="false">A18</f>
+        <v>10</v>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <f aca="false">C18</f>
+        <v>6</v>
+      </c>
+      <c r="E18" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B18,matches!$H$2:$H$199,$C18)</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B18,matches!$H$2:$H$199,$C18, matches!$F$2:$F$199, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B18,matches!$H$2:$H$199,$C18)</f>
+        <v>6</v>
+      </c>
+      <c r="H18" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B18,matches!$H$2:$H$199,$C18, matches!$F$2:$F$199, 1)</f>
+        <v>6</v>
+      </c>
+      <c r="I18" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" s="8" t="str">
+        <f aca="false">VLOOKUP(C18,all_products!$A$2:$C$13, 3, 0)</f>
+        <v>Muller Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
+      </c>
+      <c r="M18" s="8" t="str">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 4, 0)</f>
+        <v>Yogurt And White Cups</v>
+      </c>
+      <c r="N18" s="8" t="n">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 5, 0)</f>
+        <v>19</v>
+      </c>
+      <c r="O18" s="8" t="n">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 6, 0)</f>
+        <v>45</v>
+      </c>
+      <c r="P18" s="8" t="str">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 7, 0)</f>
+        <v>Central Bottling Company</v>
+      </c>
+      <c r="Q18" s="8" t="str">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 8, 0)</f>
+        <v>Yogurt and white cups</v>
+      </c>
+      <c r="R18" s="8" t="n">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 9, 0)</f>
+        <v>153</v>
+      </c>
+      <c r="S18" s="8" t="str">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 10, 0)</f>
+        <v>SKU</v>
+      </c>
+      <c r="T18" s="8" t="str">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 11, 0)</f>
+        <v>Muller Natural</v>
+      </c>
+      <c r="U18" s="8" t="n">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 12, 0)</f>
+        <v>98</v>
+      </c>
+      <c r="V18" s="8" t="n">
+        <f aca="false">VLOOKUP($C18, all_products!$A$2:$N$45, 13, 0)</f>
+        <v>7290102395224</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B19" s="8" t="n">
+        <f aca="false">A19</f>
+        <v>10</v>
+      </c>
+      <c r="C19" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D19" s="8" t="n">
+        <f aca="false">C19</f>
+        <v>7</v>
+      </c>
+      <c r="E19" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B19,matches!$H$2:$H$199,$C19)</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$199,matches!$B$2:$B$199,$B19,matches!$H$2:$H$199,$C19, matches!$F$2:$F$199, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B19,matches!$H$2:$H$199,$C19)</f>
+        <v>2</v>
+      </c>
+      <c r="H19" s="8" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$199,matches!$B$2:$B$199,$B19,matches!$H$2:$H$199,$C19, matches!$F$2:$F$199, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="I19" s="8" t="n">
+        <v>11</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="8" t="str">
+        <f aca="false">VLOOKUP(C19,all_products!$A$2:$C$13, 3, 0)</f>
+        <v>Muller 2.8% Natural Yogurt Muller Natural Cup 8 Pack x 150 ml</v>
+      </c>
+      <c r="M19" s="8" t="str">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$G$14, 4, 0)</f>
+        <v>Yogurt And White Cups</v>
+      </c>
+      <c r="N19" s="8" t="n">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$G$14, 5, 0)</f>
+        <v>19</v>
+      </c>
+      <c r="O19" s="8" t="n">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$G$14, 6, 0)</f>
+        <v>45</v>
+      </c>
+      <c r="P19" s="8" t="str">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$G$14, 7, 0)</f>
+        <v>Central Bottling Company</v>
+      </c>
+      <c r="Q19" s="8" t="str">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$L$40, 8, 0)</f>
+        <v>Yogurt and white cups</v>
+      </c>
+      <c r="R19" s="8" t="n">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$L$40, 9, 0)</f>
+        <v>153</v>
+      </c>
+      <c r="S19" s="8" t="str">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$L$40, 10, 0)</f>
+        <v>SKU</v>
+      </c>
+      <c r="T19" s="8" t="str">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$L$40, 11, 0)</f>
+        <v>Muller Natural</v>
+      </c>
+      <c r="U19" s="8" t="n">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$L$40, 12, 0)</f>
+        <v>98</v>
+      </c>
+      <c r="V19" s="8" t="n">
+        <f aca="false">VLOOKUP($C19, all_products!$A$2:$N$45, 13, 0)</f>
         <v>7290102395231</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B18" s="7" t="n">
-        <f aca="false">A18</f>
-        <v>8</v>
-      </c>
-      <c r="C18" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D18" s="7" t="n">
-        <f aca="false">C18</f>
-        <v>5</v>
-      </c>
-      <c r="E18" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B18,matches!$H$2:$H$200,$C18)</f>
-        <v>1</v>
-      </c>
-      <c r="F18" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$200,matches!$B$2:$B$200,$B18,matches!$H$2:$H$200,$C18, matches!$F$2:$F$200, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G18" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B18,matches!$H$2:$H$200,$C18)</f>
-        <v>2</v>
-      </c>
-      <c r="H18" s="7" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$200,matches!$B$2:$B$200,$B18,matches!$H$2:$H$200,$C18, matches!$F$2:$F$200, 1)</f>
-        <v>2</v>
-      </c>
-      <c r="I18" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L18" s="7" t="str">
-        <f aca="false">VLOOKUP(C18,all_products!$A$2:$C$13, 3, 0)</f>
-        <v>General Empty</v>
-      </c>
-      <c r="M18" s="7" t="str">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 4, 0)</f>
-        <v>General</v>
-      </c>
-      <c r="N18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 6, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="P18" s="7" t="str">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$G$14, 7, 0)</f>
-        <v>Other</v>
-      </c>
-      <c r="Q18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 8, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 9, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="S18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 10, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="T18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 11, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="U18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$L$40, 12, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V18" s="7" t="n">
-        <f aca="false">VLOOKUP($C18, all_products!$A$2:$N$45, 13, 0)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3197,8 +3453,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3206,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>